<commit_message>
#42 Actualización RF y nueva matriz CU-CU
- Corrección de los RF en el documento de Word, actualizando algunos, borrando otros y creando algunos nuevos.
- Actualización de la matriz de trazabilidad entre los distintos CU.
- Añadida la nueva matriz entre los CU a la memoria.

La próxima vez que me ponga con esta issue, tengo que pasar los cambios de los RF en la memoria.
</commit_message>
<xml_diff>
--- a/requeriments/v2/MatrizDeTrazabilidad CU-CU.xlsx
+++ b/requeriments/v2/MatrizDeTrazabilidad CU-CU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\aai-app\requeriments\v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BB98FD-D698-489B-B63B-540BCD3BED04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EBA369-A969-44D3-92A4-0D4E833B9534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F6415240-00A9-4DF4-9506-33D3B97BA9FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="20">
   <si>
     <t>CU-01</t>
   </si>
@@ -90,16 +90,10 @@
     <t>CU-18</t>
   </si>
   <si>
-    <t>CU-19</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
     <t>CU\CU</t>
-  </si>
-  <si>
-    <t>CU-20</t>
   </si>
 </sst>
 </file>
@@ -149,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -182,17 +176,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color auto="1"/>
@@ -221,54 +204,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color auto="1"/>
       </left>
@@ -316,21 +251,6 @@
         <color auto="1"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
         <color auto="1"/>
       </right>
       <top style="thick">
@@ -359,7 +279,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -367,46 +287,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -414,51 +316,7 @@
     <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -961,8 +819,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3313037F-F44E-47EC-A944-C5E46259723F}" name="Tabla1" displayName="Tabla1" ref="A1:U21" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
-  <autoFilter ref="A1:U21" xr:uid="{3313037F-F44E-47EC-A944-C5E46259723F}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3313037F-F44E-47EC-A944-C5E46259723F}" name="Tabla1" displayName="Tabla1" ref="A1:S19" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+  <autoFilter ref="A1:S19" xr:uid="{3313037F-F44E-47EC-A944-C5E46259723F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -982,31 +840,27 @@
     <filterColumn colId="16" hiddenButton="1"/>
     <filterColumn colId="17" hiddenButton="1"/>
     <filterColumn colId="18" hiddenButton="1"/>
-    <filterColumn colId="19" hiddenButton="1"/>
-    <filterColumn colId="20" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{B17EA7DA-DD91-4F00-9416-235FCB20D92A}" name="CU\CU" dataDxfId="20" dataCellStyle="Énfasis1"/>
-    <tableColumn id="2" xr3:uid="{EA740971-4397-4C6B-9C61-12484EB2F1DF}" name="CU-01" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{EF5CA6D8-6A12-426E-B19E-F4F93DECE625}" name="CU-02" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{B1732D14-C4F6-4D73-B91A-375747E57223}" name="CU-03" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{4CCE2DD8-704D-490D-B1AB-F126441A8C76}" name="CU-04" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{5BFF713A-F96F-4893-AD67-2680244E60E4}" name="CU-05" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{3FEE5088-992F-4268-B014-A75D3D280894}" name="CU-06" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{A0674F3A-0F38-4579-AFCF-447D5E02222A}" name="CU-07" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{E3A9CE6F-5B11-4118-8BBF-003AB9AD8E67}" name="CU-08" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{1300DDC9-9A4B-4A70-95D8-4D04F46073B3}" name="CU-09" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{E578ACB6-F5FF-4AFE-825B-F98E8A50B96B}" name="CU-10" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{F1519C5C-FD87-4E50-9BD0-B351F9562E5B}" name="CU-11" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{6F9701B2-9EDA-4B2F-85ED-6F2CF820C0BD}" name="CU-12" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{C21D18D2-8E73-4F95-B8B2-333C0FD1C464}" name="CU-13" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{6716B148-928E-4C91-A763-07F45A98C0C9}" name="CU-14" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{B100B1F8-53A0-49E3-AD1D-515E5B21ED0B}" name="CU-15" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{F4135BC6-C8AF-42A2-9ABC-C604919D2E15}" name="CU-16" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{AC83DF0A-7648-46E3-9688-61D7861F816E}" name="CU-17" dataDxfId="3"/>
-    <tableColumn id="19" xr3:uid="{DF30621D-21BC-48F8-9B02-5FF69137DD22}" name="CU-18" dataDxfId="2"/>
-    <tableColumn id="20" xr3:uid="{8D1189D8-84B4-425B-A0C7-7EB7517D6ECF}" name="CU-19" dataDxfId="1"/>
-    <tableColumn id="21" xr3:uid="{3C83132F-AA26-4B92-9CCA-BB2EB4287473}" name="CU-20" dataDxfId="0"/>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{B17EA7DA-DD91-4F00-9416-235FCB20D92A}" name="CU\CU" dataDxfId="18" dataCellStyle="Énfasis1"/>
+    <tableColumn id="2" xr3:uid="{EA740971-4397-4C6B-9C61-12484EB2F1DF}" name="CU-01" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{EF5CA6D8-6A12-426E-B19E-F4F93DECE625}" name="CU-02" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{B1732D14-C4F6-4D73-B91A-375747E57223}" name="CU-03" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{4CCE2DD8-704D-490D-B1AB-F126441A8C76}" name="CU-04" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{5BFF713A-F96F-4893-AD67-2680244E60E4}" name="CU-05" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{3FEE5088-992F-4268-B014-A75D3D280894}" name="CU-06" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{A0674F3A-0F38-4579-AFCF-447D5E02222A}" name="CU-07" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{E3A9CE6F-5B11-4118-8BBF-003AB9AD8E67}" name="CU-08" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{1300DDC9-9A4B-4A70-95D8-4D04F46073B3}" name="CU-09" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{E578ACB6-F5FF-4AFE-825B-F98E8A50B96B}" name="CU-10" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{F1519C5C-FD87-4E50-9BD0-B351F9562E5B}" name="CU-11" dataDxfId="7"/>
+    <tableColumn id="13" xr3:uid="{6F9701B2-9EDA-4B2F-85ED-6F2CF820C0BD}" name="CU-12" dataDxfId="6"/>
+    <tableColumn id="14" xr3:uid="{C21D18D2-8E73-4F95-B8B2-333C0FD1C464}" name="CU-13" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{6716B148-928E-4C91-A763-07F45A98C0C9}" name="CU-14" dataDxfId="4"/>
+    <tableColumn id="16" xr3:uid="{B100B1F8-53A0-49E3-AD1D-515E5B21ED0B}" name="CU-15" dataDxfId="3"/>
+    <tableColumn id="17" xr3:uid="{F4135BC6-C8AF-42A2-9ABC-C604919D2E15}" name="CU-16" dataDxfId="2"/>
+    <tableColumn id="18" xr3:uid="{AC83DF0A-7648-46E3-9688-61D7861F816E}" name="CU-17" dataDxfId="1"/>
+    <tableColumn id="19" xr3:uid="{DF30621D-21BC-48F8-9B02-5FF69137DD22}" name="CU-18" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1309,216 +1163,198 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7485684-9BEF-4DFE-9DF1-F1F99569A6E7}">
-  <dimension ref="A1:W54"/>
+  <dimension ref="A1:U52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="21" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="19" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="34.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:21" ht="34.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="O1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-    </row>
-    <row r="2" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+    </row>
+    <row r="2" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="U2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="W2" s="1"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="C2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" s="1"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="T3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="W3" s="1"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="U3" s="1"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1526,189 +1362,165 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="J4" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="K4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="O4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="3"/>
       <c r="Q4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U4" s="3"/>
-      <c r="W4" s="1"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S4" s="3"/>
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="I5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="M5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
+      <c r="R5" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="S5" s="3"/>
-      <c r="T5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U5" s="3"/>
-      <c r="W5" s="1"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="I6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="M6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
+      <c r="R6" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="S6" s="3"/>
-      <c r="T6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U6" s="3"/>
-      <c r="W6" s="1"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="U6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="3"/>
-      <c r="T7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U7" s="3"/>
-      <c r="W7" s="1"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="U7" s="1"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="7"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="L8" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
-      <c r="R8" s="3"/>
+      <c r="R8" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="S8" s="3"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="3"/>
-      <c r="W8" s="1"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1717,32 +1529,28 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="3"/>
+      <c r="R9" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="S9" s="3"/>
-      <c r="T9" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U9" s="3"/>
-      <c r="W9" s="1"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="U9" s="1"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="7"/>
+      <c r="B10" s="4"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1751,30 +1559,26 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
+      <c r="R10" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="S10" s="3"/>
-      <c r="T10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U10" s="3"/>
-      <c r="W10" s="1"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="7"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1784,27 +1588,25 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="L11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
+      <c r="R11" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="S11" s="3"/>
-      <c r="T11" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U11" s="3"/>
-      <c r="W11" s="1"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="U11" s="1"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="7"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1815,26 +1617,20 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
-      <c r="T12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="U12" s="3"/>
-      <c r="W12" s="1"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="U12" s="1"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="7"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1852,15 +1648,13 @@
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
-      <c r="T13" s="4"/>
-      <c r="U13" s="3"/>
-      <c r="W13" s="1"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="U13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="7"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1878,15 +1672,13 @@
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="3"/>
-      <c r="W14" s="1"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="U14" s="1"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="7"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1904,15 +1696,13 @@
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
-      <c r="T15" s="4"/>
-      <c r="U15" s="3"/>
-      <c r="W15" s="1"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="U15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="7"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -1930,15 +1720,13 @@
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="3"/>
-      <c r="W16" s="1"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="U16" s="1"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="7"/>
+      <c r="B17" s="4"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -1956,15 +1744,13 @@
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="3"/>
-      <c r="W17" s="1"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="U17" s="1"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="7"/>
+      <c r="B18" s="4"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1982,12 +1768,10 @@
       <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="3"/>
-      <c r="W18" s="1"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="U18" s="1"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="3"/>
@@ -2008,208 +1792,124 @@
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="3"/>
-      <c r="W19" s="1"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="3"/>
-      <c r="W20" s="1"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
-      <c r="T21" s="6"/>
-      <c r="U21" s="5"/>
-      <c r="V21" s="1"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="V22" s="1"/>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
+      <c r="U19" s="1"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T20" s="1"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T22" s="1"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="U27" s="1"/>
-      <c r="V27" s="1"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="U32" s="1"/>
-      <c r="V32" s="1"/>
-    </row>
-    <row r="33" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U33" s="1"/>
-      <c r="V33" s="1"/>
-    </row>
-    <row r="34" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U34" s="1"/>
-      <c r="V34" s="1"/>
-    </row>
-    <row r="35" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U35" s="1"/>
-      <c r="V35" s="1"/>
-    </row>
-    <row r="36" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U36" s="1"/>
-      <c r="V36" s="1"/>
-    </row>
-    <row r="37" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U37" s="1"/>
-      <c r="V37" s="1"/>
-    </row>
-    <row r="38" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U38" s="1"/>
-      <c r="V38" s="1"/>
-    </row>
-    <row r="39" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U39" s="1"/>
-      <c r="V39" s="1"/>
-    </row>
-    <row r="40" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U40" s="1"/>
-      <c r="V40" s="1"/>
-    </row>
-    <row r="41" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U41" s="1"/>
-      <c r="V41" s="1"/>
-    </row>
-    <row r="42" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U42" s="1"/>
-      <c r="V42" s="1"/>
-    </row>
-    <row r="43" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U43" s="1"/>
-      <c r="V43" s="1"/>
-    </row>
-    <row r="44" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U44" s="1"/>
-      <c r="V44" s="1"/>
-    </row>
-    <row r="45" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U45" s="1"/>
-      <c r="V45" s="1"/>
-    </row>
-    <row r="46" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U46" s="1"/>
-      <c r="V46" s="1"/>
-    </row>
-    <row r="47" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U47" s="1"/>
-      <c r="V47" s="1"/>
-    </row>
-    <row r="48" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U48" s="1"/>
-      <c r="V48" s="1"/>
-    </row>
-    <row r="49" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U49" s="1"/>
-      <c r="V49" s="1"/>
-    </row>
-    <row r="50" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U50" s="1"/>
-      <c r="V50" s="1"/>
-    </row>
-    <row r="51" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="U51" s="1"/>
-      <c r="V51" s="1"/>
-    </row>
-    <row r="52" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="V52" s="1"/>
-    </row>
-    <row r="53" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="V53" s="1"/>
-    </row>
-    <row r="54" spans="21:22" x14ac:dyDescent="0.25">
-      <c r="V54" s="1"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T24" s="1"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T25" s="1"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T26" s="1"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T27" s="1"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T28" s="1"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T29" s="1"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T30" s="1"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T31" s="1"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T32" s="1"/>
+    </row>
+    <row r="33" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T33" s="1"/>
+    </row>
+    <row r="34" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T34" s="1"/>
+    </row>
+    <row r="35" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T35" s="1"/>
+    </row>
+    <row r="36" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T36" s="1"/>
+    </row>
+    <row r="37" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T37" s="1"/>
+    </row>
+    <row r="38" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T38" s="1"/>
+    </row>
+    <row r="39" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T39" s="1"/>
+    </row>
+    <row r="40" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T40" s="1"/>
+    </row>
+    <row r="41" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T41" s="1"/>
+    </row>
+    <row r="42" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T42" s="1"/>
+    </row>
+    <row r="43" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T43" s="1"/>
+    </row>
+    <row r="44" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T44" s="1"/>
+    </row>
+    <row r="45" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T45" s="1"/>
+    </row>
+    <row r="46" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T46" s="1"/>
+    </row>
+    <row r="47" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T47" s="1"/>
+    </row>
+    <row r="48" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T48" s="1"/>
+    </row>
+    <row r="49" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T49" s="1"/>
+    </row>
+    <row r="50" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T50" s="1"/>
+    </row>
+    <row r="51" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T51" s="1"/>
+    </row>
+    <row r="52" spans="20:20" x14ac:dyDescent="0.25">
+      <c r="T52" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>